<commit_message>
feat(debug): fix float conversion problem
</commit_message>
<xml_diff>
--- a/输出.xlsx
+++ b/输出.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:HY96"/>
+  <dimension ref="A1:HR96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1576,41 +1576,6 @@
           <t>L_DQLJ</t>
         </is>
       </c>
-      <c r="HS1" s="1" t="inlineStr">
-        <is>
-          <t>F_BEM_JSKDPD1</t>
-        </is>
-      </c>
-      <c r="HT1" s="1" t="inlineStr">
-        <is>
-          <t>F_BEM_QtyJSCVPD1</t>
-        </is>
-      </c>
-      <c r="HU1" s="1" t="inlineStr">
-        <is>
-          <t>F_BEM_ROW_ERROR</t>
-        </is>
-      </c>
-      <c r="HV1" s="1" t="inlineStr">
-        <is>
-          <t>F_BEM_JSKDPD2</t>
-        </is>
-      </c>
-      <c r="HW1" s="1" t="inlineStr">
-        <is>
-          <t>F_BEM_QtyJSCVPD2</t>
-        </is>
-      </c>
-      <c r="HX1" s="1" t="inlineStr">
-        <is>
-          <t>F_BEM_JSKDPD3</t>
-        </is>
-      </c>
-      <c r="HY1" s="1" t="inlineStr">
-        <is>
-          <t>F_BEM_QtyJSCVPD3</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3064,27 +3029,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS3" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU3" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV3" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW3" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX3" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY3" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
@@ -3450,27 +3394,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
@@ -3857,27 +3780,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
@@ -4270,27 +4172,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT6" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX6" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
@@ -4677,27 +4558,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS7" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT7" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU7" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV7" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW7" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX7" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY7" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
@@ -5069,27 +4929,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS8" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT8" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU8" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV8" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW8" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX8" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
@@ -5455,27 +5294,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS9" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT9" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU9" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV9" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW9" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX9" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY9" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
@@ -5862,27 +5680,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS10" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT10" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU10" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV10" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW10" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX10" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
@@ -6272,27 +6069,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
@@ -6679,27 +6455,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS12" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT12" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU12" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV12" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW12" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX12" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
@@ -7083,27 +6838,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS13" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT13" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU13" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV13" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW13" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX13" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
@@ -7487,27 +7221,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS14" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT14" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU14" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV14" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW14" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX14" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY14" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
@@ -7891,27 +7604,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS15" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT15" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU15" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV15" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW15" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX15" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
@@ -8283,27 +7975,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS16" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT16" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU16" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV16" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW16" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX16" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
@@ -8666,27 +8337,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS17" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT17" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU17" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV17" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW17" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX17" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY17" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
@@ -9070,27 +8720,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS18" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT18" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU18" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV18" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW18" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX18" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
@@ -9474,27 +9103,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS19" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT19" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU19" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV19" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW19" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX19" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
@@ -9878,27 +9486,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS20" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT20" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU20" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV20" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW20" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX20" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
@@ -10300,27 +9887,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS21" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT21" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU21" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV21" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW21" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX21" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
@@ -10680,27 +10246,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS22" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT22" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU22" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV22" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW22" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX22" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
@@ -11084,27 +10629,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS23" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT23" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU23" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV23" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW23" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX23" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY23" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
@@ -11488,27 +11012,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS24" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT24" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU24" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV24" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW24" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX24" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
@@ -11873,27 +11376,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS25" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT25" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU25" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV25" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW25" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX25" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY25" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
@@ -12277,27 +11759,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS26" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT26" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU26" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV26" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW26" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX26" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY26" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
@@ -12657,27 +12118,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS27" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT27" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU27" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV27" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW27" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX27" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY27" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
@@ -13061,27 +12501,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS28" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT28" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU28" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV28" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW28" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX28" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY28" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
@@ -13465,27 +12884,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS29" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT29" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU29" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV29" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW29" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX29" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY29" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
@@ -13869,27 +13267,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS30" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT30" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU30" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV30" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW30" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX30" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY30" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
@@ -14273,27 +13650,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS31" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT31" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU31" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV31" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW31" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX31" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY31" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
@@ -14677,27 +14033,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS32" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT32" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU32" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV32" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW32" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX32" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY32" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
@@ -15081,27 +14416,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS33" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT33" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU33" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV33" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW33" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX33" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY33" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
@@ -15485,27 +14799,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS34" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT34" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU34" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV34" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW34" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX34" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY34" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
@@ -15889,27 +15182,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS35" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT35" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU35" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV35" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW35" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX35" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY35" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
@@ -16293,27 +15565,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS36" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT36" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU36" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV36" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW36" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX36" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY36" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
@@ -16697,27 +15948,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS37" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT37" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU37" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV37" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW37" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX37" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY37" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
@@ -17101,27 +16331,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS38" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT38" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU38" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV38" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW38" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX38" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY38" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
@@ -17505,27 +16714,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS39" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT39" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU39" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV39" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW39" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX39" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY39" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
@@ -17909,27 +17097,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS40" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT40" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU40" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV40" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW40" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX40" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY40" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
@@ -18306,27 +17473,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS41" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT41" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU41" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV41" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW41" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX41" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY41" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
@@ -18710,27 +17856,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS42" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT42" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU42" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV42" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW42" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX42" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY42" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
@@ -19090,27 +18215,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS43" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT43" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU43" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV43" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW43" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX43" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY43" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
@@ -19482,27 +18586,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS44" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT44" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU44" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV44" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW44" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX44" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY44" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
@@ -19886,27 +18969,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS45" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT45" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU45" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV45" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW45" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX45" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY45" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
@@ -20266,27 +19328,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS46" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT46" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU46" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV46" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW46" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX46" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY46" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="47">
       <c r="B47" t="inlineStr">
@@ -20658,27 +19699,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS47" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT47" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU47" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV47" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW47" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX47" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY47" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
@@ -21055,27 +20075,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS48" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT48" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU48" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV48" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW48" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX48" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY48" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
@@ -21447,27 +20446,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS49" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT49" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU49" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV49" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW49" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX49" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY49" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
@@ -21839,27 +20817,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS50" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT50" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU50" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV50" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW50" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX50" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY50" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
@@ -22219,27 +21176,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS51" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT51" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU51" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV51" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW51" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX51" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY51" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
@@ -22599,27 +21535,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS52" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT52" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU52" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV52" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW52" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX52" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY52" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
@@ -22979,27 +21894,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS53" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT53" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU53" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV53" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW53" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX53" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY53" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="54">
       <c r="B54" t="inlineStr">
@@ -23365,27 +22259,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS54" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT54" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU54" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV54" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW54" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX54" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY54" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="55">
       <c r="B55" t="inlineStr">
@@ -23777,27 +22650,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS55" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT55" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU55" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV55" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW55" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX55" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY55" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="56">
       <c r="B56" t="inlineStr">
@@ -24181,27 +23033,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS56" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT56" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU56" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV56" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW56" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX56" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY56" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="57">
       <c r="B57" t="inlineStr">
@@ -24585,27 +23416,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS57" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT57" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU57" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV57" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW57" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX57" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY57" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="58">
       <c r="B58" t="inlineStr">
@@ -24990,27 +23800,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS58" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT58" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU58" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV58" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW58" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX58" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY58" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="59">
       <c r="B59" t="inlineStr">
@@ -25394,27 +24183,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS59" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT59" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU59" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV59" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW59" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX59" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY59" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="60">
       <c r="B60" t="inlineStr">
@@ -25798,27 +24566,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS60" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT60" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU60" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV60" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW60" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX60" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY60" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="61">
       <c r="B61" t="inlineStr">
@@ -26202,27 +24949,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS61" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT61" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU61" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV61" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW61" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX61" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY61" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="B62" t="inlineStr">
@@ -26607,27 +25333,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS62" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT62" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU62" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV62" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW62" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX62" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY62" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
@@ -26987,27 +25692,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS63" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT63" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU63" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV63" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW63" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX63" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY63" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
@@ -27391,27 +26075,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS64" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT64" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU64" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV64" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW64" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX64" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY64" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="65">
       <c r="B65" t="inlineStr">
@@ -27771,27 +26434,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS65" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT65" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU65" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV65" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW65" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX65" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY65" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="66">
       <c r="B66" t="inlineStr">
@@ -28149,27 +26791,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS66" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT66" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU66" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV66" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW66" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX66" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY66" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="67">
       <c r="B67" t="inlineStr">
@@ -28566,27 +27187,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS67" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT67" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU67" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV67" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW67" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX67" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY67" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="68">
       <c r="B68" t="inlineStr">
@@ -28983,27 +27583,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS68" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT68" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU68" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV68" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW68" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX68" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY68" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="69">
       <c r="B69" t="inlineStr">
@@ -29369,27 +27948,6 @@
         <is>
           <t>1/2"NPT(F)</t>
         </is>
-      </c>
-      <c r="HS69" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT69" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU69" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV69" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW69" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX69" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY69" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -29894,27 +28452,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS70" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT70" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU70" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="HV70" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW70" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX70" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY70" s="4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="71">
       <c r="B71" t="inlineStr">
@@ -30298,27 +28835,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS71" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT71" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU71" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV71" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW71" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX71" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY71" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
@@ -30673,27 +29189,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS72" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT72" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU72" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV72" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW72" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX72" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY72" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
@@ -31077,27 +29572,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS73" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT73" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU73" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV73" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW73" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX73" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY73" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="74">
       <c r="B74" t="inlineStr">
@@ -31481,27 +29955,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS74" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT74" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU74" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV74" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW74" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX74" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY74" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="75">
       <c r="B75" t="inlineStr">
@@ -31885,27 +30338,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS75" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT75" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU75" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV75" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW75" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX75" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY75" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="76">
       <c r="B76" t="inlineStr">
@@ -32271,27 +30703,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS76" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT76" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU76" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV76" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW76" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX76" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY76" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
@@ -32663,27 +31074,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS77" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT77" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU77" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV77" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW77" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX77" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY77" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="78">
       <c r="B78" t="inlineStr">
@@ -33049,27 +31439,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS78" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT78" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU78" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV78" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW78" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX78" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY78" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="79">
       <c r="B79" t="inlineStr">
@@ -33441,27 +31810,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS79" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT79" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU79" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV79" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW79" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX79" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY79" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="80">
       <c r="B80" t="inlineStr">
@@ -33827,27 +32175,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS80" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT80" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU80" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV80" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW80" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX80" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY80" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="81">
       <c r="B81" t="inlineStr">
@@ -34219,27 +32546,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS81" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT81" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU81" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV81" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW81" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX81" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY81" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="82">
       <c r="B82" t="inlineStr">
@@ -34611,27 +32917,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS82" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT82" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU82" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV82" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW82" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX82" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY82" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
@@ -34991,27 +33276,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS83" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT83" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU83" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV83" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW83" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX83" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY83" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
@@ -35395,27 +33659,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS84" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT84" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU84" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV84" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW84" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX84" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY84" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="85">
       <c r="B85" t="inlineStr">
@@ -35775,27 +34018,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS85" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT85" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU85" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV85" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW85" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX85" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY85" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="86">
       <c r="B86" t="inlineStr">
@@ -36155,27 +34377,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS86" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT86" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU86" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV86" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW86" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX86" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY86" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
@@ -36559,27 +34760,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS87" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT87" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU87" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV87" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW87" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX87" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY87" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="88">
       <c r="B88" t="inlineStr">
@@ -36963,27 +35143,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS88" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT88" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU88" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV88" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW88" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX88" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY88" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
@@ -37367,27 +35526,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS89" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT89" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU89" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV89" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW89" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX89" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY89" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="90">
       <c r="B90" t="inlineStr">
@@ -37747,27 +35885,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS90" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT90" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU90" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV90" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW90" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX90" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY90" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="91">
       <c r="B91" t="inlineStr">
@@ -38152,27 +36269,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS91" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT91" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU91" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV91" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW91" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX91" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY91" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="92">
       <c r="B92" t="inlineStr">
@@ -38544,27 +36640,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS92" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT92" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU92" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV92" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW92" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX92" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY92" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="93">
       <c r="B93" t="inlineStr">
@@ -38930,27 +37005,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS93" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT93" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU93" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV93" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW93" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX93" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY93" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
@@ -39325,27 +37379,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS94" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT94" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU94" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV94" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW94" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX94" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY94" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="95">
       <c r="B95" t="inlineStr">
@@ -39732,27 +37765,6 @@
           <t>1/2"NPT(F)</t>
         </is>
       </c>
-      <c r="HS95" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT95" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU95" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV95" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW95" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX95" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY95" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
@@ -40114,27 +38126,6 @@
         <is>
           <t>1/2"NPT(F)</t>
         </is>
-      </c>
-      <c r="HS96" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT96" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU96" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV96" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW96" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX96" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY96" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>